<commit_message>
ANSYS Project, Results, PMax Calculator
Created initial ANSYS Workbench model with dynamic piston and static
weight forces as well as summary document in Design\Mechanical Analysis
Created initial Pressure/Bore Size calculator based on required leg
torque.
</commit_message>
<xml_diff>
--- a/Software/PressureBoreCalc.xlsx
+++ b/Software/PressureBoreCalc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="15">
   <si>
     <t>Torque [N-m]</t>
   </si>
@@ -60,16 +60,32 @@
   </si>
   <si>
     <t>Knee</t>
+  </si>
+  <si>
+    <t>Max Knee Acc</t>
+  </si>
+  <si>
+    <t>Max Hip Acc</t>
+  </si>
+  <si>
+    <t>Avg Knee Acc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,13 +178,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H14"/>
+  <dimension ref="A2:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,187 +482,677 @@
     <col min="7" max="7" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="J4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4">
+      <c r="J5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6">
         <v>195</v>
       </c>
-      <c r="C4">
-        <f>B4*8.85</f>
+      <c r="C6">
+        <f>B6*8.85</f>
         <v>1725.75</v>
       </c>
-      <c r="D4">
-        <f>3.149*2</f>
-        <v>6.298</v>
-      </c>
-      <c r="E4">
-        <f>C4/D4</f>
-        <v>274.01556049539533</v>
-      </c>
-      <c r="F4">
+      <c r="D6">
+        <f>3.149*1</f>
+        <v>3.149</v>
+      </c>
+      <c r="E6">
+        <f>C6/D6</f>
+        <v>548.03112099079067</v>
+      </c>
+      <c r="F6">
         <v>2.5</v>
       </c>
-      <c r="G4">
-        <f>PI()*(F4/2)^2</f>
+      <c r="G6">
+        <f>PI()*(F6/2)^2</f>
         <v>4.908738521234052</v>
       </c>
-      <c r="H4" s="1">
-        <f>E4/G4</f>
-        <v>55.821991599281212</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="F6" t="s">
+      <c r="H6" s="1">
+        <f>E6/G6</f>
+        <v>111.64398319856242</v>
+      </c>
+      <c r="J6">
+        <v>118</v>
+      </c>
+      <c r="K6">
+        <f>J6*8.85</f>
+        <v>1044.3</v>
+      </c>
+      <c r="L6">
+        <f>3.149*4</f>
+        <v>12.596</v>
+      </c>
+      <c r="M6">
+        <f>K6/L6</f>
+        <v>82.907272149888854</v>
+      </c>
+      <c r="N6">
+        <v>2.5</v>
+      </c>
+      <c r="O6">
+        <f>PI()*(N6/2)^2</f>
+        <v>4.908738521234052</v>
+      </c>
+      <c r="P6" s="1">
+        <f>M6/O6</f>
+        <v>16.889730791577396</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
         <v>7</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G8" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="F7">
+      <c r="N8" t="s">
+        <v>7</v>
+      </c>
+      <c r="O8" t="s">
+        <v>8</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F9">
         <v>100</v>
       </c>
-      <c r="G7">
-        <f>E4/F7</f>
-        <v>2.7401556049539533</v>
-      </c>
-      <c r="H7" s="2">
-        <f>SQRT(G7/PI())*2</f>
-        <v>1.867852905063746</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="3" t="s">
+      <c r="G9">
+        <f>E6/F9</f>
+        <v>5.4803112099079065</v>
+      </c>
+      <c r="H9" s="2">
+        <f>SQRT(G9/PI())*2</f>
+        <v>2.6415429108591351</v>
+      </c>
+      <c r="N9">
+        <v>100</v>
+      </c>
+      <c r="O9">
+        <f>M6/N9</f>
+        <v>0.82907272149888855</v>
+      </c>
+      <c r="P9" s="2">
+        <f>SQRT(O9/PI())*2</f>
+        <v>1.0274279412560217</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="5"/>
+      <c r="J11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>0</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E12" t="s">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F12" t="s">
         <v>4</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G12" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11">
+      <c r="J12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" t="s">
+        <v>5</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>27</v>
       </c>
-      <c r="C11">
-        <f>B11*8.85</f>
+      <c r="C13">
+        <f>B13*8.85</f>
         <v>238.95</v>
       </c>
-      <c r="D11">
-        <f>3.149*2</f>
-        <v>6.298</v>
-      </c>
-      <c r="E11">
-        <f>C11/D11</f>
-        <v>37.940616068593201</v>
-      </c>
-      <c r="F11">
+      <c r="D13">
+        <f>3.149*1</f>
+        <v>3.149</v>
+      </c>
+      <c r="E13">
+        <f>C13/D13</f>
+        <v>75.881232137186402</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <f>PI()*(F13/2)^2</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="H13" s="1">
+        <f>E13/G13</f>
+        <v>24.153746365073605</v>
+      </c>
+      <c r="J13">
+        <v>275</v>
+      </c>
+      <c r="K13">
+        <f>J13*8.85</f>
+        <v>2433.75</v>
+      </c>
+      <c r="L13">
+        <f>3.149*4</f>
+        <v>12.596</v>
+      </c>
+      <c r="M13">
+        <f>K13/L13</f>
+        <v>193.21610034931723</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <f>PI()*(N13/2)^2</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="P13" s="1">
+        <f>M13/O13</f>
+        <v>61.50259491106705</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" t="s">
+        <v>7</v>
+      </c>
+      <c r="O15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>100</v>
+      </c>
+      <c r="G16">
+        <f>E13/F16</f>
+        <v>0.75881232137186405</v>
+      </c>
+      <c r="H16" s="2">
+        <f>SQRT(G16/PI())*2</f>
+        <v>0.98292922156325391</v>
+      </c>
+      <c r="N16">
+        <v>100</v>
+      </c>
+      <c r="O16">
+        <f>M13/N16</f>
+        <v>1.9321610034931722</v>
+      </c>
+      <c r="P16" s="2">
+        <f>SQRT(O16/PI())*2</f>
+        <v>1.5684718028841582</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="J19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="J21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="5"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="J22" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22" t="s">
+        <v>2</v>
+      </c>
+      <c r="M22" t="s">
+        <v>3</v>
+      </c>
+      <c r="N22" t="s">
+        <v>4</v>
+      </c>
+      <c r="O22" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="J23">
+        <v>60</v>
+      </c>
+      <c r="K23">
+        <f>J23*8.85</f>
+        <v>531</v>
+      </c>
+      <c r="L23">
+        <f>3.149*4</f>
+        <v>12.596</v>
+      </c>
+      <c r="M23">
+        <f>K23/L23</f>
+        <v>42.156240076214672</v>
+      </c>
+      <c r="N23">
         <v>2.5</v>
       </c>
-      <c r="G11">
-        <f>PI()*(F11/2)^2</f>
+      <c r="O23">
+        <f>PI()*(N23/2)^2</f>
         <v>4.908738521234052</v>
       </c>
-      <c r="H11" s="1">
-        <f>E11/G11</f>
-        <v>7.7291988368235529</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="F13" t="s">
+      <c r="P23" s="1">
+        <f>M23/O23</f>
+        <v>8.5879987075817255</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="N25" t="s">
         <v>7</v>
       </c>
-      <c r="G13" t="s">
+      <c r="O25" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="F14">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="N26">
         <v>100</v>
       </c>
-      <c r="G14">
-        <f>E11/F14</f>
-        <v>0.37940616068593203</v>
-      </c>
-      <c r="H14" s="2">
-        <f>SQRT(G14/PI())*2</f>
-        <v>0.69503591799379127</v>
-      </c>
+      <c r="O26">
+        <f>M23/N26</f>
+        <v>0.42156240076214674</v>
+      </c>
+      <c r="P26" s="2">
+        <f>SQRT(O26/PI())*2</f>
+        <v>0.73263218549546261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="J28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="J29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K29" t="s">
+        <v>1</v>
+      </c>
+      <c r="L29" t="s">
+        <v>2</v>
+      </c>
+      <c r="M29" t="s">
+        <v>3</v>
+      </c>
+      <c r="N29" t="s">
+        <v>4</v>
+      </c>
+      <c r="O29" t="s">
+        <v>5</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="J30">
+        <v>47</v>
+      </c>
+      <c r="K30">
+        <f>J30*8.85</f>
+        <v>415.95</v>
+      </c>
+      <c r="L30">
+        <f>3.149*4</f>
+        <v>12.596</v>
+      </c>
+      <c r="M30">
+        <f>K30/L30</f>
+        <v>33.022388059701491</v>
+      </c>
+      <c r="N30">
+        <v>2</v>
+      </c>
+      <c r="O30">
+        <f>PI()*(N30/2)^2</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="P30" s="1">
+        <f>M30/O30</f>
+        <v>10.51135258480055</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="P31" s="1"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="N32" t="s">
+        <v>7</v>
+      </c>
+      <c r="O32" t="s">
+        <v>8</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="N33">
+        <v>100</v>
+      </c>
+      <c r="O33">
+        <f>M30/N33</f>
+        <v>0.33022388059701491</v>
+      </c>
+      <c r="P33" s="2">
+        <f>SQRT(O33/PI())*2</f>
+        <v>0.648424323565998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed values to be more realistic in pneumatic calculator
Used matlab parameters and a generic 100 PSI air compressor to calculate
values along with a generic pneumatic cylinder with approximate values.
</commit_message>
<xml_diff>
--- a/Software/PressureBoreCalc.xlsx
+++ b/Software/PressureBoreCalc.xlsx
@@ -786,12 +786,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -807,9 +801,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -841,15 +832,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -862,15 +844,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -882,15 +855,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -904,27 +868,12 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -953,9 +902,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -985,13 +931,67 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1278,7 +1278,7 @@
   <dimension ref="B1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1298,39 +1298,39 @@
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="8"/>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="24">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="13"/>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="F4" s="80" t="s">
+      <c r="D4" s="95"/>
+      <c r="F4" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="82"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="99"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="16"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="15" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="83" t="s">
+      <c r="F5" s="68" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="12" t="s">
@@ -1345,116 +1345,118 @@
       <c r="J5" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="84" t="s">
+      <c r="K5" s="69" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="9">
-        <v>195</v>
-      </c>
-      <c r="D6" s="19">
-        <v>27</v>
+        <v>334</v>
+      </c>
+      <c r="D6" s="17">
+        <v>37</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="F6" s="89">
+      <c r="F6" s="72">
         <f>'Pressure Calculations'!H6</f>
-        <v>174.44372374775381</v>
-      </c>
-      <c r="G6" s="90">
+        <v>58.827443165599</v>
+      </c>
+      <c r="G6" s="73">
         <f>'Pressure Calculations'!H13</f>
-        <v>24.153746365073605</v>
-      </c>
-      <c r="H6" s="91">
+        <v>14.119760560206148</v>
+      </c>
+      <c r="H6" s="74">
         <f>'Volumetric Flow Calculations'!J7</f>
-        <v>8.3792725387410414</v>
-      </c>
-      <c r="I6" s="91">
+        <v>6.6838331969411726</v>
+      </c>
+      <c r="I6" s="74">
         <f>'Volumetric Flow Calculations'!J11</f>
-        <v>0.86063159668531464</v>
-      </c>
-      <c r="J6" s="100">
+        <v>1.9648426227031359</v>
+      </c>
+      <c r="J6" s="82">
         <f>I6+H6</f>
-        <v>9.2399041354263556</v>
-      </c>
-      <c r="K6" s="101">
+        <v>8.6486758196443088</v>
+      </c>
+      <c r="K6" s="83">
         <f>MAX(F6:G6)</f>
-        <v>174.44372374775381</v>
+        <v>58.827443165599</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="9">
-        <v>118</v>
-      </c>
-      <c r="D7" s="19">
-        <v>275</v>
+        <v>26</v>
+      </c>
+      <c r="D7" s="17">
+        <v>75</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="89">
+      <c r="F7" s="72">
         <f>'Pressure Calculations'!P6</f>
-        <v>105.56081744735872</v>
-      </c>
-      <c r="G7" s="90">
+        <v>4.5793818033101017</v>
+      </c>
+      <c r="G7" s="73">
         <f>'Pressure Calculations'!P13</f>
-        <v>246.0103796442682</v>
-      </c>
-      <c r="H7" s="91">
+        <v>28.621136270688137</v>
+      </c>
+      <c r="H7" s="74">
         <f>'Volumetric Flow Calculations'!J16</f>
-        <v>5.3276849221129359</v>
-      </c>
-      <c r="I7" s="91">
+        <v>1.7525452615460584</v>
+      </c>
+      <c r="I7" s="74">
         <f>'Volumetric Flow Calculations'!J20</f>
-        <v>5.7748765896968086</v>
-      </c>
-      <c r="J7" s="100">
+        <v>2.9535018110493962</v>
+      </c>
+      <c r="J7" s="82">
         <f>I7+H7</f>
-        <v>11.102561511809744</v>
-      </c>
-      <c r="K7" s="101">
+        <v>4.7060470725954548</v>
+      </c>
+      <c r="K7" s="83">
         <f t="shared" ref="K7:K8" si="0">MAX(F7:G7)</f>
-        <v>246.0103796442682</v>
+        <v>28.621136270688137</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="21">
-        <v>60</v>
-      </c>
-      <c r="D8" s="22">
-        <v>47</v>
+      <c r="C8" s="19">
+        <f>AVERAGE(24.6, 5.1, 14.8, 5.11)</f>
+        <v>12.4025</v>
+      </c>
+      <c r="D8" s="20">
+        <f>AVERAGE(11.3, 9.4, 30.4, 9.4)</f>
+        <v>15.125</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="92">
+      <c r="F8" s="75">
         <f>'Pressure Calculations'!P23</f>
-        <v>53.674991922385793</v>
-      </c>
-      <c r="G8" s="93">
+        <v>2.1844531852135973</v>
+      </c>
+      <c r="G8" s="76">
         <f>'Pressure Calculations'!P30</f>
-        <v>42.045410339202199</v>
-      </c>
-      <c r="H8" s="94">
+        <v>5.7719291479221067</v>
+      </c>
+      <c r="H8" s="77">
         <f>'Volumetric Flow Calculations'!J25</f>
-        <v>3.0290864576398171</v>
-      </c>
-      <c r="I8" s="94">
+        <v>1.5348401066709445</v>
+      </c>
+      <c r="I8" s="77">
         <f>'Volumetric Flow Calculations'!J29</f>
-        <v>1.2569416767668866</v>
-      </c>
-      <c r="J8" s="102">
+        <v>1.3957131557274922</v>
+      </c>
+      <c r="J8" s="84">
         <f>I8+H8</f>
-        <v>4.2860281344067035</v>
-      </c>
-      <c r="K8" s="103">
+        <v>2.9305532623984369</v>
+      </c>
+      <c r="K8" s="85">
         <f t="shared" si="0"/>
-        <v>53.674991922385793</v>
+        <v>5.7719291479221067</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
@@ -1464,136 +1466,138 @@
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="F11" s="85" t="s">
+      <c r="D11" s="95"/>
+      <c r="F11" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="86"/>
-      <c r="I11" s="85" t="s">
+      <c r="G11" s="101"/>
+      <c r="I11" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="J11" s="97"/>
-      <c r="K11" s="86"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="101"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="87" t="s">
+      <c r="F12" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="88" t="s">
+      <c r="G12" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="87" t="s">
+      <c r="I12" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="J12" s="98" t="s">
+      <c r="J12" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="K12" s="99" t="s">
+      <c r="K12" s="81" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="25">
-        <v>2</v>
-      </c>
-      <c r="D13" s="32">
-        <v>2</v>
-      </c>
-      <c r="F13" s="95">
+      <c r="C13" s="22">
+        <v>2.5</v>
+      </c>
+      <c r="D13" s="29">
+        <v>2.5</v>
+      </c>
+      <c r="F13" s="78">
         <v>2.6</v>
       </c>
-      <c r="G13" s="96">
+      <c r="G13" s="79">
         <v>6</v>
       </c>
-      <c r="I13" s="104">
+      <c r="I13" s="86">
         <f>J8-F13</f>
-        <v>1.6860281344067034</v>
-      </c>
-      <c r="J13" s="102">
+        <v>0.33055326239843685</v>
+      </c>
+      <c r="J13" s="84">
         <f>(I13*14.7)/(MAX(K6:K8)+14.7)</f>
-        <v>9.5065695541529383E-2</v>
-      </c>
-      <c r="K13" s="105">
+        <v>6.6085977535125906E-2</v>
+      </c>
+      <c r="K13" s="87">
         <f>G13/J13</f>
-        <v>63.11424921283939</v>
+        <v>90.790818624282139</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="28" t="s">
         <v>25</v>
       </c>
       <c r="I14" s="11"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C15" s="25">
-        <v>3.149</v>
-      </c>
-      <c r="D15" s="32">
-        <v>3.149</v>
+      <c r="C15" s="22">
+        <f>0.393701*26</f>
+        <v>10.236226</v>
+      </c>
+      <c r="D15" s="22">
+        <f>0.393701*12</f>
+        <v>4.7244120000000001</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="28" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="29">
+      <c r="C17" s="26">
+        <v>8</v>
+      </c>
+      <c r="D17" s="30">
         <v>6</v>
       </c>
-      <c r="D17" s="33">
-        <v>3</v>
-      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="31" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="35">
-        <v>0.2</v>
-      </c>
-      <c r="D19" s="36">
-        <v>0.2</v>
+      <c r="C19" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="33">
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="106" t="s">
+      <c r="B24" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="107"/>
-      <c r="D24" s="107"/>
-      <c r="E24" s="107"/>
-      <c r="F24" s="108"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="90"/>
     </row>
     <row r="25" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="111" t="s">
+      <c r="B25" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="109"/>
-      <c r="D25" s="109"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="110"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="92"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1617,7 +1621,7 @@
   <dimension ref="A2:Q35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1705,87 +1709,87 @@
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6">
         <f>Main!C6</f>
-        <v>195</v>
+        <v>334</v>
       </c>
       <c r="C6">
         <f>B6*8.85</f>
-        <v>1725.75</v>
+        <v>2955.9</v>
       </c>
       <c r="D6">
         <f>Main!C15</f>
-        <v>3.149</v>
+        <v>10.236226</v>
       </c>
       <c r="E6">
         <f>C6/D6</f>
-        <v>548.03112099079067</v>
+        <v>288.76853637268266</v>
       </c>
       <c r="F6">
         <f>Main!C13</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="G6">
         <f>PI()*(F6/2)^2</f>
-        <v>3.1415926535897931</v>
+        <v>4.908738521234052</v>
       </c>
       <c r="H6" s="1">
         <f>E6/G6</f>
-        <v>174.44372374775381</v>
+        <v>58.827443165599</v>
       </c>
       <c r="J6">
         <f>Main!C7</f>
-        <v>118</v>
+        <v>26</v>
       </c>
       <c r="K6">
         <f>J6*8.85</f>
-        <v>1044.3</v>
+        <v>230.1</v>
       </c>
       <c r="L6">
         <f>Main!C15</f>
-        <v>3.149</v>
+        <v>10.236226</v>
       </c>
       <c r="M6">
         <f>K6/L6</f>
-        <v>331.62908859955542</v>
+        <v>22.478987861346553</v>
       </c>
       <c r="N6">
         <f>Main!C13</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="O6">
         <f>PI()*(N6/2)^2</f>
-        <v>3.1415926535897931</v>
+        <v>4.908738521234052</v>
       </c>
       <c r="P6" s="1">
         <f>M6/O6</f>
-        <v>105.56081744735872</v>
+        <v>4.5793818033101017</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="F7" s="5"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
       <c r="I7" s="5"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="F8" s="5"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
       <c r="I8" s="5"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="F9" s="5"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
       <c r="I9" s="5"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
     </row>
     <row r="10" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1855,100 +1859,100 @@
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13">
         <f>Main!D6</f>
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <f>B13*8.85</f>
-        <v>238.95</v>
+        <v>327.45</v>
       </c>
       <c r="D13">
         <f>Main!D15</f>
-        <v>3.149</v>
+        <v>4.7244120000000001</v>
       </c>
       <c r="E13">
         <f>C13/D13</f>
-        <v>75.881232137186402</v>
+        <v>69.310212572485213</v>
       </c>
       <c r="F13">
         <f>Main!D13</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="G13">
         <f>PI()*(F13/2)^2</f>
-        <v>3.1415926535897931</v>
+        <v>4.908738521234052</v>
       </c>
       <c r="H13" s="1">
         <f>E13/G13</f>
-        <v>24.153746365073605</v>
+        <v>14.119760560206148</v>
       </c>
       <c r="J13">
         <f>Main!D7</f>
-        <v>275</v>
+        <v>75</v>
       </c>
       <c r="K13">
         <f>J13*8.85</f>
-        <v>2433.75</v>
+        <v>663.75</v>
       </c>
       <c r="L13">
         <f>Main!D15</f>
-        <v>3.149</v>
+        <v>4.7244120000000001</v>
       </c>
       <c r="M13">
         <f>K13/L13</f>
-        <v>772.86440139726892</v>
+        <v>140.49367413341596</v>
       </c>
       <c r="N13">
         <f>Main!D13</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="O13">
         <f>PI()*(N13/2)^2</f>
-        <v>3.1415926535897931</v>
+        <v>4.908738521234052</v>
       </c>
       <c r="P13" s="1">
         <f>M13/O13</f>
-        <v>246.0103796442682</v>
+        <v>28.621136270688137</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="26"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="26"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
@@ -1957,8 +1961,8 @@
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
       <c r="J19" t="s">
         <v>11</v>
       </c>
@@ -2034,31 +2038,31 @@
       <c r="H23" s="6"/>
       <c r="J23">
         <f>Main!C8</f>
-        <v>60</v>
+        <v>12.4025</v>
       </c>
       <c r="K23">
         <f>J23*8.85</f>
-        <v>531</v>
+        <v>109.762125</v>
       </c>
       <c r="L23">
         <f>Main!C15</f>
-        <v>3.149</v>
+        <v>10.236226</v>
       </c>
       <c r="M23">
         <f>K23/L23</f>
-        <v>168.62496030485869</v>
+        <v>10.722909498090409</v>
       </c>
       <c r="N23">
         <f>Main!C13</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="O23">
         <f>PI()*(N23/2)^2</f>
-        <v>3.1415926535897931</v>
+        <v>4.908738521234052</v>
       </c>
       <c r="P23" s="1">
         <f>M23/O23</f>
-        <v>53.674991922385793</v>
+        <v>2.1844531852135973</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
@@ -2070,11 +2074,11 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
@@ -2085,11 +2089,11 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
@@ -2100,11 +2104,11 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
-      <c r="Q26" s="26"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
     </row>
     <row r="27" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
@@ -2177,31 +2181,31 @@
       <c r="H30" s="6"/>
       <c r="J30">
         <f>Main!D8</f>
-        <v>47</v>
+        <v>15.125</v>
       </c>
       <c r="K30">
         <f>J30*8.85</f>
-        <v>415.95</v>
+        <v>133.85624999999999</v>
       </c>
       <c r="L30">
         <f>Main!D15</f>
-        <v>3.149</v>
+        <v>4.7244120000000001</v>
       </c>
       <c r="M30">
         <f>K30/L30</f>
-        <v>132.08955223880596</v>
+        <v>28.332890950238884</v>
       </c>
       <c r="N30">
         <f>Main!D13</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="O30">
         <f>PI()*(N30/2)^2</f>
-        <v>3.1415926535897931</v>
+        <v>4.908738521234052</v>
       </c>
       <c r="P30" s="1">
         <f>M30/O30</f>
-        <v>42.045410339202199</v>
+        <v>5.7719291479221067</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
@@ -2213,11 +2217,11 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
-      <c r="Q31" s="26"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23"/>
+      <c r="Q31" s="23"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
@@ -2228,11 +2232,11 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
-      <c r="M32" s="26"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="26"/>
-      <c r="Q32" s="26"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
@@ -2243,11 +2247,11 @@
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="26"/>
-      <c r="Q33" s="26"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
@@ -2295,515 +2299,515 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
     </row>
     <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="105"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
     </row>
     <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="55"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="46"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="57" t="s">
+      <c r="D6" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="57" t="s">
+      <c r="F6" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="57" t="s">
+      <c r="H6" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="57" t="s">
+      <c r="I6" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="58" t="s">
+      <c r="J6" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="59">
+      <c r="B7" s="50">
         <f>Main!$C$17</f>
-        <v>6</v>
-      </c>
-      <c r="C7" s="60">
+        <v>8</v>
+      </c>
+      <c r="C7" s="51">
         <f>Main!$C$13</f>
-        <v>2</v>
-      </c>
-      <c r="D7" s="60">
+        <v>2.5</v>
+      </c>
+      <c r="D7" s="51">
         <f>Main!$C$19</f>
-        <v>0.2</v>
-      </c>
-      <c r="E7" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="51">
         <f>1/(Main!$E$2/60)</f>
         <v>30</v>
       </c>
-      <c r="F7" s="60">
+      <c r="F7" s="51">
         <f>PI()*C7^2/4</f>
-        <v>3.1415926535897931</v>
-      </c>
-      <c r="G7" s="60">
+        <v>4.908738521234052</v>
+      </c>
+      <c r="G7" s="51">
         <f>PI()*D7^2/4</f>
-        <v>3.1415926535897934E-2</v>
-      </c>
-      <c r="H7" s="60">
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="H7" s="51">
         <f>((2*F7-G7)*B7*E7)/(12^3)</f>
-        <v>0.65122597715038422</v>
-      </c>
-      <c r="I7" s="60">
+        <v>1.3362677085581589</v>
+      </c>
+      <c r="I7" s="51">
         <f>Main!F6</f>
-        <v>174.44372374775381</v>
-      </c>
-      <c r="J7" s="78">
+        <v>58.827443165599</v>
+      </c>
+      <c r="J7" s="66">
         <f>H7*(I7+14.7)/14.7</f>
-        <v>8.3792725387410414</v>
-      </c>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
+        <v>6.6838331969411726</v>
+      </c>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
     </row>
     <row r="8" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="56"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
     </row>
     <row r="9" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="57" t="s">
+      <c r="D10" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="57" t="s">
+      <c r="G10" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="57" t="s">
+      <c r="H10" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="57" t="s">
+      <c r="I10" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="58" t="s">
+      <c r="J10" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
     </row>
     <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="62">
+      <c r="B11" s="53">
         <f>Main!$D$17</f>
-        <v>3</v>
-      </c>
-      <c r="C11" s="63">
+        <v>6</v>
+      </c>
+      <c r="C11" s="54">
         <f>Main!$D$13</f>
-        <v>2</v>
-      </c>
-      <c r="D11" s="63">
+        <v>2.5</v>
+      </c>
+      <c r="D11" s="54">
         <f>Main!$D$19</f>
-        <v>0.2</v>
-      </c>
-      <c r="E11" s="63">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="54">
         <f>1/(Main!$E$2/60)</f>
         <v>30</v>
       </c>
-      <c r="F11" s="63">
+      <c r="F11" s="54">
         <f>PI()*C11^2/4</f>
-        <v>3.1415926535897931</v>
-      </c>
-      <c r="G11" s="63">
+        <v>4.908738521234052</v>
+      </c>
+      <c r="G11" s="54">
         <f>PI()*D11^2/4</f>
-        <v>3.1415926535897934E-2</v>
-      </c>
-      <c r="H11" s="63">
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="H11" s="54">
         <f>((2*F11-G11)*B11*E11)/(12^3)</f>
-        <v>0.32561298857519211</v>
-      </c>
-      <c r="I11" s="63">
+        <v>1.0022007814186189</v>
+      </c>
+      <c r="I11" s="54">
         <f>Main!G6</f>
-        <v>24.153746365073605</v>
-      </c>
-      <c r="J11" s="79">
+        <v>14.119760560206148</v>
+      </c>
+      <c r="J11" s="67">
         <f>H11*(I11+14.7)/14.7</f>
-        <v>0.86063159668531464</v>
-      </c>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="26"/>
+        <v>1.9648426227031359</v>
+      </c>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
     </row>
     <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
     </row>
     <row r="13" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="66"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="107"/>
+      <c r="F13" s="107"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="107"/>
+      <c r="I13" s="107"/>
+      <c r="J13" s="108"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
     </row>
     <row r="14" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="69"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="57"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="71" t="s">
+      <c r="C15" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="71" t="s">
+      <c r="D15" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="71" t="s">
+      <c r="E15" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="71" t="s">
+      <c r="F15" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="71" t="s">
+      <c r="G15" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="H15" s="71" t="s">
+      <c r="H15" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="71" t="s">
+      <c r="I15" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="J15" s="72" t="s">
+      <c r="J15" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="26"/>
-      <c r="R15" s="26"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="73">
+      <c r="B16" s="61">
         <f>Main!$C$17</f>
-        <v>6</v>
-      </c>
-      <c r="C16" s="74">
+        <v>8</v>
+      </c>
+      <c r="C16" s="62">
         <f>Main!$C$13</f>
-        <v>2</v>
-      </c>
-      <c r="D16" s="74">
+        <v>2.5</v>
+      </c>
+      <c r="D16" s="62">
         <f>Main!$C$19</f>
-        <v>0.2</v>
-      </c>
-      <c r="E16" s="74">
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="62">
         <f>1/(Main!$E$2/60)</f>
         <v>30</v>
       </c>
-      <c r="F16" s="74">
+      <c r="F16" s="62">
         <f>PI()*C16^2/4</f>
-        <v>3.1415926535897931</v>
-      </c>
-      <c r="G16" s="74">
+        <v>4.908738521234052</v>
+      </c>
+      <c r="G16" s="62">
         <f>PI()*D16^2/4</f>
-        <v>3.1415926535897934E-2</v>
-      </c>
-      <c r="H16" s="74">
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="H16" s="62">
         <f>((2*F16-G16)*B16*E16)/(12^3)</f>
-        <v>0.65122597715038422</v>
-      </c>
-      <c r="I16" s="74">
+        <v>1.3362677085581589</v>
+      </c>
+      <c r="I16" s="62">
         <f>Main!F7</f>
-        <v>105.56081744735872</v>
-      </c>
-      <c r="J16" s="78">
+        <v>4.5793818033101017</v>
+      </c>
+      <c r="J16" s="66">
         <f>H16*(I16+14.7)/14.7</f>
-        <v>5.3276849221129359</v>
-      </c>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
+        <v>1.7525452615460584</v>
+      </c>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
     </row>
     <row r="17" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="70"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="75"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="63"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
     </row>
     <row r="18" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="69"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="26"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="57"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B19" s="70" t="s">
+      <c r="B19" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="71" t="s">
+      <c r="C19" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="71" t="s">
+      <c r="D19" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="71" t="s">
+      <c r="E19" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="71" t="s">
+      <c r="F19" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="71" t="s">
+      <c r="G19" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="71" t="s">
+      <c r="H19" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="I19" s="71" t="s">
+      <c r="I19" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="J19" s="72" t="s">
+      <c r="J19" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="26"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
     </row>
     <row r="20" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="76">
+      <c r="B20" s="64">
         <f>Main!$D$17</f>
-        <v>3</v>
-      </c>
-      <c r="C20" s="77">
+        <v>6</v>
+      </c>
+      <c r="C20" s="65">
         <f>Main!$D$13</f>
-        <v>2</v>
-      </c>
-      <c r="D20" s="77">
+        <v>2.5</v>
+      </c>
+      <c r="D20" s="65">
         <f>Main!$D$19</f>
-        <v>0.2</v>
-      </c>
-      <c r="E20" s="77">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="65">
         <f>1/(Main!$E$2/60)</f>
         <v>30</v>
       </c>
-      <c r="F20" s="77">
+      <c r="F20" s="65">
         <f>PI()*C20^2/4</f>
-        <v>3.1415926535897931</v>
-      </c>
-      <c r="G20" s="77">
+        <v>4.908738521234052</v>
+      </c>
+      <c r="G20" s="65">
         <f>PI()*D20^2/4</f>
-        <v>3.1415926535897934E-2</v>
-      </c>
-      <c r="H20" s="77">
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="H20" s="65">
         <f>((2*F20-G20)*B20*E20)/(12^3)</f>
-        <v>0.32561298857519211</v>
-      </c>
-      <c r="I20" s="77">
+        <v>1.0022007814186189</v>
+      </c>
+      <c r="I20" s="65">
         <f>Main!G7</f>
-        <v>246.0103796442682</v>
-      </c>
-      <c r="J20" s="79">
+        <v>28.621136270688137</v>
+      </c>
+      <c r="J20" s="67">
         <f>H20*(I20+14.7)/14.7</f>
-        <v>5.7748765896968086</v>
-      </c>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="26"/>
+        <v>2.9535018110493962</v>
+      </c>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
     </row>
     <row r="21" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="6"/>
@@ -2815,253 +2819,253 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="26"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
     </row>
     <row r="22" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="39"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
+      <c r="C22" s="110"/>
+      <c r="D22" s="110"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="110"/>
+      <c r="G22" s="110"/>
+      <c r="H22" s="110"/>
+      <c r="I22" s="110"/>
+      <c r="J22" s="111"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
     </row>
     <row r="23" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="42"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="26"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="36"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="44" t="s">
+      <c r="E24" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="44" t="s">
+      <c r="F24" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="G24" s="44" t="s">
+      <c r="G24" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="H24" s="44" t="s">
+      <c r="H24" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="I24" s="44" t="s">
+      <c r="I24" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="J24" s="45" t="s">
+      <c r="J24" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B25" s="46">
+      <c r="B25" s="40">
         <f>Main!$C$17</f>
-        <v>6</v>
-      </c>
-      <c r="C25" s="47">
+        <v>8</v>
+      </c>
+      <c r="C25" s="41">
         <f>Main!$C$13</f>
-        <v>2</v>
-      </c>
-      <c r="D25" s="47">
+        <v>2.5</v>
+      </c>
+      <c r="D25" s="41">
         <f>Main!$C$19</f>
-        <v>0.2</v>
-      </c>
-      <c r="E25" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="41">
         <f>1/(Main!$E$2/60)</f>
         <v>30</v>
       </c>
-      <c r="F25" s="47">
+      <c r="F25" s="41">
         <f>PI()*C25^2/4</f>
-        <v>3.1415926535897931</v>
-      </c>
-      <c r="G25" s="47">
+        <v>4.908738521234052</v>
+      </c>
+      <c r="G25" s="41">
         <f>PI()*D25^2/4</f>
-        <v>3.1415926535897934E-2</v>
-      </c>
-      <c r="H25" s="47">
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="H25" s="41">
         <f>((2*F25-G25)*B25*E25)/(12^3)</f>
-        <v>0.65122597715038422</v>
-      </c>
-      <c r="I25" s="47">
+        <v>1.3362677085581589</v>
+      </c>
+      <c r="I25" s="41">
         <f>Main!F8</f>
-        <v>53.674991922385793</v>
-      </c>
-      <c r="J25" s="78">
+        <v>2.1844531852135973</v>
+      </c>
+      <c r="J25" s="66">
         <f>H25*(I25+14.7)/14.7</f>
-        <v>3.0290864576398171</v>
-      </c>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
+        <v>1.5348401066709445</v>
+      </c>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
     </row>
     <row r="26" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="43"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="48"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
-      <c r="Q26" s="26"/>
-      <c r="R26" s="26"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="42"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="23"/>
     </row>
     <row r="27" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="42"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="26"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="36"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="44" t="s">
+      <c r="D28" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="44" t="s">
+      <c r="E28" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="44" t="s">
+      <c r="F28" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="44" t="s">
+      <c r="G28" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="H28" s="44" t="s">
+      <c r="H28" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="I28" s="44" t="s">
+      <c r="I28" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="J28" s="45" t="s">
+      <c r="J28" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
-      <c r="Q28" s="26"/>
-      <c r="R28" s="26"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
     </row>
     <row r="29" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="30">
+      <c r="B29" s="27">
         <f>Main!$D$17</f>
-        <v>3</v>
-      </c>
-      <c r="C29" s="49">
+        <v>6</v>
+      </c>
+      <c r="C29" s="43">
         <f>Main!$D$13</f>
-        <v>2</v>
-      </c>
-      <c r="D29" s="49">
+        <v>2.5</v>
+      </c>
+      <c r="D29" s="43">
         <f>Main!$D$19</f>
-        <v>0.2</v>
-      </c>
-      <c r="E29" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="43">
         <f>1/(Main!$E$2/60)</f>
         <v>30</v>
       </c>
-      <c r="F29" s="49">
+      <c r="F29" s="43">
         <f>PI()*C29^2/4</f>
-        <v>3.1415926535897931</v>
-      </c>
-      <c r="G29" s="49">
+        <v>4.908738521234052</v>
+      </c>
+      <c r="G29" s="43">
         <f>PI()*D29^2/4</f>
-        <v>3.1415926535897934E-2</v>
-      </c>
-      <c r="H29" s="49">
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="H29" s="43">
         <f>((2*F29-G29)*B29*E29)/(12^3)</f>
-        <v>0.32561298857519211</v>
-      </c>
-      <c r="I29" s="49">
+        <v>1.0022007814186189</v>
+      </c>
+      <c r="I29" s="43">
         <f>Main!G8</f>
-        <v>42.045410339202199</v>
-      </c>
-      <c r="J29" s="79">
+        <v>5.7719291479221067</v>
+      </c>
+      <c r="J29" s="67">
         <f>H29*(I29+14.7)/14.7</f>
-        <v>1.2569416767668866</v>
-      </c>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="26"/>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="26"/>
+        <v>1.3957131557274922</v>
+      </c>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B30" s="6"/>
@@ -3073,13 +3077,13 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
-      <c r="Q30" s="26"/>
-      <c r="R30" s="26"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="23"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B31" s="6"/>
@@ -3091,13 +3095,13 @@
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
-      <c r="Q31" s="26"/>
-      <c r="R31" s="26"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23"/>
+      <c r="Q31" s="23"/>
+      <c r="R31" s="23"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B32" s="6"/>
@@ -3109,13 +3113,13 @@
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="26"/>
-      <c r="Q32" s="26"/>
-      <c r="R32" s="26"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B33" s="6"/>
@@ -3127,13 +3131,13 @@
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="26"/>
-      <c r="Q33" s="26"/>
-      <c r="R33" s="26"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="23"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B34" s="6"/>
@@ -3145,13 +3149,13 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
-      <c r="Q34" s="26"/>
-      <c r="R34" s="26"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Converting gallon to ft3
</commit_message>
<xml_diff>
--- a/Software/PressureBoreCalc.xlsx
+++ b/Software/PressureBoreCalc.xlsx
@@ -1278,7 +1278,7 @@
   <dimension ref="B1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1525,8 +1525,8 @@
         <v>6.6085977535125906E-2</v>
       </c>
       <c r="K13" s="87">
-        <f>G13/J13</f>
-        <v>90.790818624282139</v>
+        <f>(G13*0.134)/J13</f>
+        <v>12.165969695653807</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
@@ -2284,7 +2284,7 @@
   <dimension ref="B3:R34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Weekly to do list update
</commit_message>
<xml_diff>
--- a/Software/PressureBoreCalc.xlsx
+++ b/Software/PressureBoreCalc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -1301,8 +1301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1523,7 +1523,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="78">
-        <v>2.6</v>
+        <v>1.5</v>
       </c>
       <c r="G13" s="92">
         <v>8</v>
@@ -1588,15 +1588,15 @@
       </c>
       <c r="G18" s="86">
         <f>J8-F13</f>
-        <v>-0.17396579908097243</v>
+        <v>0.92603420091902766</v>
       </c>
       <c r="H18" s="84">
         <f>(G18*14.7)/(H13+14.7)</f>
-        <v>-1.8985131748257569E-2</v>
+        <v>0.10105941168158655</v>
       </c>
       <c r="I18" s="87">
         <f>(G13*0.134)/H18</f>
-        <v>-56.465238915099278</v>
+        <v>10.607621617446274</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1647,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>